<commit_message>
Fixed. works with .xls docs
</commit_message>
<xml_diff>
--- a/uploads/TestData.xlsx
+++ b/uploads/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15795" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -146,6 +146,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -477,12 +482,12 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>123456</v>
       </c>
@@ -522,7 +527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>123455</v>
       </c>
@@ -542,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>123454</v>
       </c>
@@ -562,7 +567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>123453</v>
       </c>
@@ -582,7 +587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>123452</v>
       </c>
@@ -602,7 +607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>123451</v>
       </c>

</xml_diff>